<commit_message>
Not found & bouton "Voir la fiche"
</commit_message>
<xml_diff>
--- a/private/TABLE DE CORRESPONDANCE 27 09 2016 - Famille 1 - BIS.xlsx
+++ b/private/TABLE DE CORRESPONDANCE 27 09 2016 - Famille 1 - BIS.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="138">
   <si>
     <t xml:space="preserve">TABLES DE CORRESPONDANCE HACKATHON</t>
   </si>
@@ -418,9 +418,6 @@
     <t xml:space="preserve">Non applicable</t>
   </si>
   <si>
-    <t xml:space="preserve">Radical de compte d'alerte 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Libellé d'alerte 3</t>
   </si>
   <si>
@@ -463,7 +460,7 @@
     <t xml:space="preserve">6711 ou 6712</t>
   </si>
   <si>
-    <t xml:space="preserve">Pas 6712 ou 6712</t>
+    <t xml:space="preserve">Pas 6711 ou 6712</t>
   </si>
   <si>
     <t xml:space="preserve">Pas 7717</t>
@@ -512,7 +509,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -656,12 +653,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -883,7 +874,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -972,10 +963,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.3117408906883"/>
-    <col collapsed="false" hidden="false" max="10" min="2" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="36.3117408906883"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="10" min="2" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -1553,10 +1544,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.3117408906883"/>
-    <col collapsed="false" hidden="false" max="10" min="2" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="36.3117408906883"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="10" min="2" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -2154,11 +2145,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.3117408906883"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.6356275303644"/>
     <col collapsed="false" hidden="true" max="6" min="2" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="36.3117408906883"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -2836,13 +2827,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.3117408906883"/>
-    <col collapsed="false" hidden="false" max="10" min="2" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.9595141700405"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="10" min="2" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="28.1740890688259"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -3684,11 +3675,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.3117408906883"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="10" min="7" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="23" min="11" style="0" width="36.3117408906883"/>
+    <col collapsed="false" hidden="false" max="23" min="11" style="0" width="36.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -4748,12 +4739,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.4898785425101"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.8097165991903"/>
     <col collapsed="false" hidden="true" max="16" min="2" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="22" min="19" style="0" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="36.3117408906883"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="22" min="19" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="36.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -6061,29 +6052,25 @@
   </sheetPr>
   <dimension ref="A1:AL42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3570" ySplit="1095" topLeftCell="N1" activePane="bottomRight" state="split"/>
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="topRight" activeCell="N3" activeCellId="0" sqref="N3"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomRight" activeCell="S27" activeCellId="0" sqref="S27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="7" min="2" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="16" min="14" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="27.9595141700405"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="25" min="24" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="27" min="26" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="38" min="28" style="0" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="2" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="16" min="14" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.1740890688259"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="25" min="24" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="27" min="26" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="38" min="28" style="0" width="32.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="39" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -6776,7 +6763,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="33"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -6811,10 +6798,8 @@
       <c r="AK12" s="6"/>
       <c r="AL12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="33" t="s">
-        <v>110</v>
-      </c>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="33"/>
       <c r="B13" s="6" t="s">
         <v>109</v>
       </c>
@@ -7281,7 +7266,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>109</v>
@@ -7424,7 +7409,7 @@
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>15</v>
@@ -7575,7 +7560,7 @@
     </row>
     <row r="23" s="36" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B23" s="35" t="s">
         <v>109</v>
@@ -7614,13 +7599,13 @@
         <v>58</v>
       </c>
       <c r="N23" s="36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O23" s="36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P23" s="36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q23" s="35" t="s">
         <v>60</v>
@@ -7630,28 +7615,28 @@
       </c>
       <c r="S23" s="35"/>
       <c r="T23" s="35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U23" s="35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="V23" s="35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="W23" s="35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="X23" s="35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Y23" s="35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Z23" s="35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AA23" s="35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AB23" s="35" t="s">
         <v>93</v>
@@ -7660,31 +7645,31 @@
         <v>93</v>
       </c>
       <c r="AD23" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE23" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF23" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG23" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="AE23" s="37" t="s">
+      <c r="AH23" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="AF23" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG23" s="35" t="s">
+      <c r="AI23" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="AH23" s="35" t="s">
+      <c r="AJ23" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="AI23" s="35" t="s">
+      <c r="AK23" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="AJ23" s="35" t="s">
+      <c r="AL23" s="35" t="s">
         <v>118</v>
-      </c>
-      <c r="AK23" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="AL23" s="35" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7724,7 +7709,7 @@
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>109</v>
@@ -7766,10 +7751,10 @@
         <v>63</v>
       </c>
       <c r="O25" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="P25" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="P25" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="Q25" s="5" t="s">
         <v>62</v>
@@ -7784,25 +7769,25 @@
         <v>63514</v>
       </c>
       <c r="U25" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="V25" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="V25" s="24" t="s">
+      <c r="W25" s="24" t="s">
         <v>124</v>
-      </c>
-      <c r="W25" s="24" t="s">
-        <v>125</v>
       </c>
       <c r="X25" s="24" t="n">
         <v>7717</v>
       </c>
       <c r="Y25" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Z25" s="24" t="n">
         <v>649</v>
       </c>
       <c r="AA25" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AB25" s="6" t="s">
         <v>63</v>
@@ -7814,10 +7799,10 @@
         <v>63</v>
       </c>
       <c r="AE25" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF25" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="AF25" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="AG25" s="6" t="s">
         <v>63</v>
@@ -7908,7 +7893,7 @@
         <v>109</v>
       </c>
       <c r="AC27" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AD27" s="6" t="s">
         <v>109</v>
@@ -7923,24 +7908,24 @@
         <v>109</v>
       </c>
       <c r="AH27" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AI27" s="6" t="s">
         <v>109</v>
       </c>
       <c r="AJ27" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AK27" s="6" t="s">
         <v>109</v>
       </c>
       <c r="AL27" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -7964,37 +7949,37 @@
       <c r="Z28" s="24"/>
       <c r="AA28" s="24"/>
       <c r="AB28" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC28" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="AC28" s="6" t="s">
-        <v>131</v>
-      </c>
       <c r="AD28" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="AE28" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="AE28" s="6" t="s">
-        <v>131</v>
-      </c>
       <c r="AF28" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AG28" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="AH28" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="AH28" s="6" t="s">
-        <v>131</v>
-      </c>
       <c r="AI28" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="AJ28" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="AJ28" s="6" t="s">
-        <v>131</v>
-      </c>
       <c r="AK28" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="AL28" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="AL28" s="6" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8036,115 +8021,115 @@
         <v>18</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F30" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="G30" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="H30" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="I30" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="J30" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="K30" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="L30" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="O30" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="P30" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q30" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="R30" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="S30" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="T30" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="U30" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="V30" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="W30" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="X30" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y30" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z30" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA30" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB30" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC30" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD30" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE30" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="AF30" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="H30" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="I30" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="J30" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="K30" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="L30" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="M30" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="N30" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="O30" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="P30" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q30" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="R30" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="S30" s="38" t="s">
+      <c r="AG30" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH30" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="AI30" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ30" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="AK30" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL30" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="T30" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="U30" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="V30" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="W30" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="X30" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y30" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="Z30" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA30" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="AB30" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC30" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="AD30" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="AE30" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="AF30" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="AG30" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="AH30" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="AI30" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ30" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="AK30" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="AL30" s="6" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8220,7 +8205,7 @@
         <v>65</v>
       </c>
       <c r="P32" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q32" s="6" t="s">
         <v>67</v>
@@ -8247,13 +8232,13 @@
         <v>109</v>
       </c>
       <c r="Y32" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Z32" s="6" t="s">
         <v>109</v>
       </c>
       <c r="AA32" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AB32" s="6" t="s">
         <v>109</v>
@@ -8274,7 +8259,7 @@
         <v>109</v>
       </c>
       <c r="AH32" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AI32" s="6" t="s">
         <v>109</v>
@@ -8337,7 +8322,7 @@
         <v>23</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>36</v>
@@ -8376,19 +8361,19 @@
         <v>109</v>
       </c>
       <c r="S34" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="T34" s="6" t="s">
         <v>109</v>
       </c>
       <c r="U34" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="V34" s="6" t="s">
         <v>109</v>
       </c>
       <c r="W34" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="X34" s="6" t="s">
         <v>109</v>
@@ -8406,7 +8391,7 @@
         <v>109</v>
       </c>
       <c r="AC34" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AD34" s="6" t="s">
         <v>109</v>
@@ -8427,7 +8412,7 @@
         <v>109</v>
       </c>
       <c r="AJ34" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AK34" s="6" t="s">
         <v>109</v>

</xml_diff>